<commit_message>
gender, fee-paying and location by postcode
</commit_message>
<xml_diff>
--- a/schools.xlsx
+++ b/schools.xlsx
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">funding</t>
-  </si>
-  <si>
     <t xml:space="preserve">postcode</t>
   </si>
   <si>
@@ -43,6 +37,12 @@
     <t xml:space="preserve">contact_number</t>
   </si>
   <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eton</t>
   </si>
   <si>
@@ -55,18 +55,33 @@
     <t xml:space="preserve">0800 00 1066</t>
   </si>
   <si>
+    <t xml:space="preserve">private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
     <t xml:space="preserve">Waterloo Road</t>
   </si>
   <si>
     <t xml:space="preserve">LU5 5PX</t>
   </si>
   <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co-ed</t>
+  </si>
+  <si>
     <t xml:space="preserve">school1</t>
   </si>
   <si>
     <t xml:space="preserve">B44 8DT</t>
   </si>
   <si>
+    <t xml:space="preserve">utc</t>
+  </si>
+  <si>
     <t xml:space="preserve">school2</t>
   </si>
   <si>
@@ -92,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">GL7 1ZT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
   </si>
   <si>
     <t xml:space="preserve">school6</t>
@@ -122,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -143,6 +161,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -198,6 +221,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -220,10 +247,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.9"/>
   </cols>
@@ -255,188 +282,188 @@
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>200</v>
+      <c r="B2" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1000000</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="n">
         <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="C4" s="0" t="n">
-        <v>3498</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>305</v>
+        <v>20</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>20934</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>10000000</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>823756</v>
+        <v>7</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="0" t="n">
         <v>1234567989</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>3478</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="0" t="n">
         <v>9</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>39</v>
+        <v>27</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>123478</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="0" t="n">
         <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>34678</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="0" t="n">
         <v>14</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>124</v>
+        <v>32</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>97654</v>
+        <v>19</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="0" t="n">
         <v>7745989056</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>257234</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>